<commit_message>
Added information regarding the Molex Header
</commit_message>
<xml_diff>
--- a/03 BOM/Fan - Electrical BOM.xlsx
+++ b/03 BOM/Fan - Electrical BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Balsamo\Documents\Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D822AAD2-3849-47D5-89C0-8DAF2B9F54A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A369136-6D50-4666-AD6E-CB9AAFC1623B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE7979A0-422C-4BD6-A3E3-FA281A28C7D7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Fan Control Board Bill of Materials</t>
   </si>
@@ -77,12 +77,6 @@
     <t>SPDT</t>
   </si>
   <si>
-    <t>5pin molex</t>
-  </si>
-  <si>
-    <t>2pin molex</t>
-  </si>
-  <si>
     <t>Power Supply</t>
   </si>
   <si>
@@ -96,13 +90,46 @@
   </si>
   <si>
     <t>* Optional</t>
+  </si>
+  <si>
+    <t>Connectors</t>
+  </si>
+  <si>
+    <t>5pin molex (SL)</t>
+  </si>
+  <si>
+    <t>2pin molex (SL)</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Mate</t>
+  </si>
+  <si>
+    <t>Crimp</t>
+  </si>
+  <si>
+    <t>0050579405</t>
+  </si>
+  <si>
+    <t>0050579402</t>
+  </si>
+  <si>
+    <t>0016020103</t>
+  </si>
+  <si>
+    <t>0705430004</t>
+  </si>
+  <si>
+    <t>0705430001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +139,23 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -154,10 +198,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,16 +230,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>132486</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>170774</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>46761</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>85049</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -211,7 +262,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2600325" y="285750"/>
+          <a:off x="4953000" y="390525"/>
           <a:ext cx="6914286" cy="5409524"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -521,107 +572,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64472E74-4988-4FA6-8014-7D2FD9BA4513}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>